<commit_message>
update algorithms_aitype excel file
</commit_message>
<xml_diff>
--- a/database/excel_tables/individual_tables/algorithms_aitype.xlsx
+++ b/database/excel_tables/individual_tables/algorithms_aitype.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="251">
   <si>
     <t>algorithms</t>
   </si>
@@ -82,6 +82,9 @@
     <t>bpnn</t>
   </si>
   <si>
+    <t>canfis</t>
+  </si>
+  <si>
     <t>ccnn</t>
   </si>
   <si>
@@ -124,6 +127,12 @@
     <t>gdalbnn</t>
   </si>
   <si>
+    <t>gmdh</t>
+  </si>
+  <si>
+    <t>grnn</t>
+  </si>
+  <si>
     <t>gru</t>
   </si>
   <si>
@@ -298,285 +307,276 @@
     <t>shap-xgboost</t>
   </si>
   <si>
+    <t>custom fuzzy logic algorithm</t>
+  </si>
+  <si>
+    <t>fahp</t>
+  </si>
+  <si>
+    <t>mamdani</t>
+  </si>
+  <si>
+    <t>sfc</t>
+  </si>
+  <si>
+    <t>xfuzzy3.0</t>
+  </si>
+  <si>
+    <t>bert</t>
+  </si>
+  <si>
+    <t>chatgpt</t>
+  </si>
+  <si>
+    <t>gpt models</t>
+  </si>
+  <si>
+    <t>gpt-2</t>
+  </si>
+  <si>
+    <t>gpt3</t>
+  </si>
+  <si>
+    <t>open ai models</t>
+  </si>
+  <si>
+    <t>gwr</t>
+  </si>
+  <si>
+    <t>mgrw</t>
+  </si>
+  <si>
+    <t>regression kriging</t>
+  </si>
+  <si>
+    <t>ggcn</t>
+  </si>
+  <si>
+    <t>hybrid reasoning</t>
+  </si>
+  <si>
+    <t>cbr</t>
+  </si>
+  <si>
+    <t>chatbots</t>
+  </si>
+  <si>
+    <t>dssat</t>
+  </si>
+  <si>
+    <t>lpo</t>
+  </si>
+  <si>
+    <t>microleis dss</t>
+  </si>
+  <si>
+    <t>mha</t>
+  </si>
+  <si>
+    <t>mas custom algorithm</t>
+  </si>
+  <si>
+    <t>slam</t>
+  </si>
+  <si>
+    <t>ahp</t>
+  </si>
+  <si>
+    <t>crm</t>
+  </si>
+  <si>
+    <t>dematel</t>
+  </si>
+  <si>
+    <t>electre</t>
+  </si>
+  <si>
+    <t>maut</t>
+  </si>
+  <si>
+    <t>mcoa</t>
+  </si>
+  <si>
+    <t>topsis</t>
+  </si>
+  <si>
+    <t>custom nlp algorithm</t>
+  </si>
+  <si>
+    <t>lexalytics</t>
+  </si>
+  <si>
+    <t>ner</t>
+  </si>
+  <si>
+    <t>nltk</t>
+  </si>
+  <si>
+    <t>cgda</t>
+  </si>
+  <si>
+    <t>cgpb</t>
+  </si>
+  <si>
+    <t>lma</t>
+  </si>
+  <si>
+    <t>moo</t>
+  </si>
+  <si>
+    <t>muzo</t>
+  </si>
+  <si>
+    <t>sop</t>
+  </si>
+  <si>
+    <t>nau</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>bayesian algorithm</t>
+  </si>
+  <si>
+    <t>blwl</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>bnm</t>
+  </si>
+  <si>
+    <t>bra</t>
+  </si>
+  <si>
+    <t>cdrm</t>
+  </si>
+  <si>
+    <t>garch</t>
+  </si>
+  <si>
+    <t>mcs</t>
+  </si>
+  <si>
+    <t>ddqn</t>
+  </si>
+  <si>
+    <t>q-learning</t>
+  </si>
+  <si>
+    <t>rl custom algorithm</t>
+  </si>
+  <si>
+    <t>rn</t>
+  </si>
+  <si>
+    <t>sarsa</t>
+  </si>
+  <si>
+    <t>stdn</t>
+  </si>
+  <si>
+    <t>ablwl</t>
+  </si>
+  <si>
+    <t>adaboost</t>
+  </si>
+  <si>
+    <t>arma</t>
+  </si>
+  <si>
+    <t>brt</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>catboost</t>
+  </si>
+  <si>
+    <t>decision tree</t>
+  </si>
+  <si>
+    <t>emla</t>
+  </si>
+  <si>
+    <t>ensemble learning</t>
+  </si>
+  <si>
+    <t>fda</t>
+  </si>
+  <si>
+    <t>gbm</t>
+  </si>
+  <si>
+    <t>gpr</t>
+  </si>
+  <si>
+    <t>id3</t>
+  </si>
+  <si>
+    <t>knn</t>
+  </si>
+  <si>
+    <t>lightgbm</t>
+  </si>
+  <si>
+    <t>linear regression</t>
+  </si>
+  <si>
+    <t>logistic regression</t>
+  </si>
+  <si>
+    <t>lsm</t>
+  </si>
+  <si>
+    <t>lsqb</t>
+  </si>
+  <si>
+    <t>lssvm</t>
+  </si>
+  <si>
+    <t>lwlr</t>
+  </si>
+  <si>
+    <t>mars</t>
+  </si>
+  <si>
+    <t>mblwl</t>
+  </si>
+  <si>
+    <t>mca</t>
+  </si>
+  <si>
+    <t>mkl</t>
+  </si>
+  <si>
+    <t>mlc</t>
+  </si>
+  <si>
+    <t>mlr</t>
+  </si>
+  <si>
+    <t>mpmr</t>
+  </si>
+  <si>
     <t>mrmr</t>
   </si>
   <si>
+    <t>multiple regression</t>
+  </si>
+  <si>
+    <t>mvlr</t>
+  </si>
+  <si>
     <t>nca</t>
   </si>
   <si>
     <t>ncda</t>
   </si>
   <si>
-    <t>canfis</t>
-  </si>
-  <si>
-    <t>custom fuzzy logic algorithm</t>
-  </si>
-  <si>
-    <t>fahp</t>
-  </si>
-  <si>
-    <t>mamdani</t>
-  </si>
-  <si>
-    <t>sfc</t>
-  </si>
-  <si>
-    <t>xfuzzy3.0</t>
-  </si>
-  <si>
-    <t>bert</t>
-  </si>
-  <si>
-    <t>chatgpt</t>
-  </si>
-  <si>
-    <t>gpt models</t>
-  </si>
-  <si>
-    <t>gpt-2</t>
-  </si>
-  <si>
-    <t>gpt3</t>
-  </si>
-  <si>
-    <t>open ai models</t>
-  </si>
-  <si>
-    <t>gwr</t>
-  </si>
-  <si>
-    <t>mgrw</t>
-  </si>
-  <si>
-    <t>regression kriging</t>
-  </si>
-  <si>
-    <t>ggcn</t>
-  </si>
-  <si>
-    <t>hybrid reasoning</t>
-  </si>
-  <si>
-    <t>cbr</t>
-  </si>
-  <si>
-    <t>chatbots</t>
-  </si>
-  <si>
-    <t>dssat</t>
-  </si>
-  <si>
-    <t>lpo</t>
-  </si>
-  <si>
-    <t>microleis dss</t>
-  </si>
-  <si>
-    <t>ablwl</t>
-  </si>
-  <si>
-    <t>mblwl</t>
-  </si>
-  <si>
-    <t>mha</t>
-  </si>
-  <si>
-    <t>mas custom algorithm</t>
-  </si>
-  <si>
-    <t>slam</t>
-  </si>
-  <si>
-    <t>ahp</t>
-  </si>
-  <si>
-    <t>crm</t>
-  </si>
-  <si>
-    <t>dematel</t>
-  </si>
-  <si>
-    <t>electre</t>
-  </si>
-  <si>
-    <t>maut</t>
-  </si>
-  <si>
-    <t>mcoa</t>
-  </si>
-  <si>
-    <t>topsis</t>
-  </si>
-  <si>
-    <t>gmdh</t>
-  </si>
-  <si>
-    <t>grnn</t>
-  </si>
-  <si>
-    <t>custom nlp algorithm</t>
-  </si>
-  <si>
-    <t>lexalytics</t>
-  </si>
-  <si>
-    <t>ner</t>
-  </si>
-  <si>
-    <t>nltk</t>
-  </si>
-  <si>
-    <t>cgda</t>
-  </si>
-  <si>
-    <t>cgpb</t>
-  </si>
-  <si>
-    <t>lma</t>
-  </si>
-  <si>
-    <t>moo</t>
-  </si>
-  <si>
-    <t>muzo</t>
-  </si>
-  <si>
-    <t>sop</t>
-  </si>
-  <si>
-    <t>nau</t>
-  </si>
-  <si>
-    <t>overall</t>
-  </si>
-  <si>
-    <t>blwl</t>
-  </si>
-  <si>
-    <t>bra</t>
-  </si>
-  <si>
-    <t>ddqn</t>
-  </si>
-  <si>
-    <t>q-learning</t>
-  </si>
-  <si>
-    <t>rl custom algorithm</t>
-  </si>
-  <si>
-    <t>rn</t>
-  </si>
-  <si>
-    <t>sarsa</t>
-  </si>
-  <si>
-    <t>stdn</t>
-  </si>
-  <si>
-    <t>bayesian algorithm</t>
-  </si>
-  <si>
-    <t>bn</t>
-  </si>
-  <si>
-    <t>bnm</t>
-  </si>
-  <si>
-    <t>cdrm</t>
-  </si>
-  <si>
-    <t>garch</t>
-  </si>
-  <si>
-    <t>mcs</t>
-  </si>
-  <si>
-    <t>adaboost</t>
-  </si>
-  <si>
-    <t>arma</t>
-  </si>
-  <si>
-    <t>brt</t>
-  </si>
-  <si>
-    <t>cart</t>
-  </si>
-  <si>
-    <t>catboost</t>
-  </si>
-  <si>
-    <t>decision tree</t>
-  </si>
-  <si>
-    <t>emla</t>
-  </si>
-  <si>
-    <t>ensemble learning</t>
-  </si>
-  <si>
-    <t>fda</t>
-  </si>
-  <si>
-    <t>gbm</t>
-  </si>
-  <si>
-    <t>gpr</t>
-  </si>
-  <si>
-    <t>id3</t>
-  </si>
-  <si>
-    <t>knn</t>
-  </si>
-  <si>
-    <t>lightgbm</t>
-  </si>
-  <si>
-    <t>linear regression</t>
-  </si>
-  <si>
-    <t>logistic regression</t>
-  </si>
-  <si>
-    <t>lsm</t>
-  </si>
-  <si>
-    <t>lsqb</t>
-  </si>
-  <si>
-    <t>lssvm</t>
-  </si>
-  <si>
-    <t>lwlr</t>
-  </si>
-  <si>
-    <t>mars</t>
-  </si>
-  <si>
-    <t>mca</t>
-  </si>
-  <si>
-    <t>mkl</t>
-  </si>
-  <si>
-    <t>mlc</t>
-  </si>
-  <si>
-    <t>mlr</t>
-  </si>
-  <si>
-    <t>mpmr</t>
-  </si>
-  <si>
-    <t>multiple regression</t>
-  </si>
-  <si>
-    <t>mvlr</t>
-  </si>
-  <si>
     <t>non-linear regression</t>
   </si>
   <si>
@@ -709,9 +709,6 @@
     <t>explainable ai</t>
   </si>
   <si>
-    <t>feature selection and dimensionality reduction</t>
-  </si>
-  <si>
     <t>fuzzy logic</t>
   </si>
   <si>
@@ -733,9 +730,6 @@
     <t>llm</t>
   </si>
   <si>
-    <t>local learning</t>
-  </si>
-  <si>
     <t>metaheuristics</t>
   </si>
   <si>
@@ -745,16 +739,13 @@
     <t>multi-criteria decision making ai</t>
   </si>
   <si>
-    <t>neural networks</t>
-  </si>
-  <si>
     <t>nlp</t>
   </si>
   <si>
     <t>optimization algorithms</t>
   </si>
   <si>
-    <t>probabilistic models</t>
+    <t>probabilistic reasoning</t>
   </si>
   <si>
     <t>reinforcement learning</t>
@@ -766,9 +757,6 @@
     <t>spatio-temporal ai</t>
   </si>
   <si>
-    <t>statistical and probabilistic models</t>
-  </si>
-  <si>
     <t>supervised machine learning</t>
   </si>
   <si>
@@ -776,9 +764,6 @@
   </si>
   <si>
     <t>symbolic ai</t>
-  </si>
-  <si>
-    <t>time series analysis</t>
   </si>
   <si>
     <t>unsupervised machine learning</t>
@@ -1139,7 +1124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B264"/>
+  <dimension ref="A1:B260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1427,7 +1412,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>227</v>
@@ -1435,7 +1420,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>227</v>
@@ -1555,7 +1540,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>227</v>
@@ -1563,7 +1548,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>227</v>
@@ -1571,7 +1556,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>227</v>
@@ -1579,7 +1564,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
         <v>227</v>
@@ -1611,7 +1596,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>227</v>
@@ -1619,7 +1604,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
         <v>227</v>
@@ -1627,7 +1612,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>227</v>
@@ -1635,7 +1620,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
         <v>227</v>
@@ -1643,7 +1628,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
         <v>227</v>
@@ -1651,34 +1636,34 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1686,7 +1671,7 @@
         <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1694,7 +1679,7 @@
         <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1702,7 +1687,7 @@
         <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>229</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1710,7 +1695,7 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>229</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1718,7 +1703,7 @@
         <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1918,7 +1903,7 @@
         <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1926,20 +1911,20 @@
         <v>91</v>
       </c>
       <c r="B98" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="B99" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B100" t="s">
         <v>230</v>
@@ -1947,7 +1932,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B101" t="s">
         <v>230</v>
@@ -1955,10 +1940,10 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1966,7 +1951,7 @@
         <v>95</v>
       </c>
       <c r="B103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1974,7 +1959,7 @@
         <v>96</v>
       </c>
       <c r="B104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1982,151 +1967,151 @@
         <v>18</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="B106" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B111" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B112" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B114" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B115" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B116" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B117" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B120" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B121" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B122" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B123" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2134,108 +2119,108 @@
         <v>18</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B126" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B127" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B129" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B130" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B131" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B132" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B133" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B134" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B135" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B136" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="B137" t="s">
         <v>239</v>
@@ -2243,234 +2228,234 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B138" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B139" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B140" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B141" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B142" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B143" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B144" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B145" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="B146" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B147" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="B148" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B149" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="B150" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B151" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B152" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="B153" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="B154" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="B155" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B156" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B157" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B158" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="B159" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="B160" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>137</v>
+        <v>55</v>
       </c>
       <c r="B161" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B162" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>138</v>
+      </c>
+      <c r="B163" t="s">
         <v>139</v>
-      </c>
-      <c r="B163" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B164" t="s">
-        <v>245</v>
+        <v>139</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B165" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B166" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2478,7 +2463,7 @@
         <v>142</v>
       </c>
       <c r="B167" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2486,7 +2471,7 @@
         <v>143</v>
       </c>
       <c r="B168" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2494,7 +2479,7 @@
         <v>144</v>
       </c>
       <c r="B169" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2502,7 +2487,7 @@
         <v>145</v>
       </c>
       <c r="B170" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2510,7 +2495,7 @@
         <v>146</v>
       </c>
       <c r="B171" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2518,7 +2503,7 @@
         <v>147</v>
       </c>
       <c r="B172" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2526,7 +2511,7 @@
         <v>148</v>
       </c>
       <c r="B173" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2534,7 +2519,7 @@
         <v>149</v>
       </c>
       <c r="B174" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2542,7 +2527,7 @@
         <v>150</v>
       </c>
       <c r="B175" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2550,39 +2535,39 @@
         <v>151</v>
       </c>
       <c r="B176" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="B177" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="B178" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="B179" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="B180" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2590,7 +2575,7 @@
         <v>154</v>
       </c>
       <c r="B181" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2598,7 +2583,7 @@
         <v>155</v>
       </c>
       <c r="B182" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2606,103 +2591,103 @@
         <v>156</v>
       </c>
       <c r="B183" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B184" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B185" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="B186" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B187" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B188" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B189" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B190" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B191" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B192" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B193" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B194" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="B195" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2710,7 +2695,7 @@
         <v>166</v>
       </c>
       <c r="B196" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2718,7 +2703,7 @@
         <v>167</v>
       </c>
       <c r="B197" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2726,7 +2711,7 @@
         <v>168</v>
       </c>
       <c r="B198" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2734,79 +2719,79 @@
         <v>169</v>
       </c>
       <c r="B199" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="B200" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B201" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B202" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B203" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B204" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B205" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B206" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B207" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
       <c r="B208" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2814,7 +2799,7 @@
         <v>178</v>
       </c>
       <c r="B209" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2822,438 +2807,406 @@
         <v>179</v>
       </c>
       <c r="B210" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B211" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B212" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>110</v>
+        <v>182</v>
       </c>
       <c r="B213" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B214" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B215" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B216" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B217" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B218" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B219" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B220" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B221" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B222" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B223" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B224" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B225" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B226" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B227" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B228" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>196</v>
+        <v>96</v>
       </c>
       <c r="B229" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B230" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
       <c r="B231" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B232" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B233" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B234" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B235" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B236" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B237" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
       <c r="B238" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>131</v>
+        <v>206</v>
       </c>
       <c r="B240" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>113</v>
+        <v>207</v>
       </c>
       <c r="B241" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B242" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B243" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B244" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B245" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B246" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
       <c r="B247" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>46</v>
+        <v>213</v>
       </c>
       <c r="B248" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="B249" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B250" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="B251" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B252" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B253" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B254" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B255" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B256" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="B257" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B258" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B259" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B260" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2">
-      <c r="A261" t="s">
-        <v>11</v>
-      </c>
-      <c r="B261" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2">
-      <c r="A262" t="s">
-        <v>222</v>
-      </c>
-      <c r="B262" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2">
-      <c r="A263" t="s">
-        <v>223</v>
-      </c>
-      <c r="B263" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
-      <c r="A264" t="s">
-        <v>224</v>
-      </c>
-      <c r="B264" t="s">
         <v>224</v>
       </c>
     </row>

</xml_diff>